<commit_message>
Added merged names and subjects data to normalize, and small edit to an OLR
</commit_message>
<xml_diff>
--- a/datamares/OLR/OLR_datamares_ecosystems.xlsx
+++ b/datamares/OLR/OLR_datamares_ecosystems.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\datamares\Working_Metadata\Batch_2_ecosystems_2016-10-14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\datamares\OLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="0" windowWidth="21600" windowHeight="10545"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="21600" windowHeight="10545" tabRatio="408"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="691">
   <si>
     <t>text</t>
   </si>
@@ -3437,12 +3437,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomLeft" activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3469,10 +3469,9 @@
     <col min="23" max="23" width="34.85546875" style="25" customWidth="1"/>
     <col min="24" max="25" width="42.85546875" style="3" customWidth="1"/>
     <col min="26" max="26" width="59.28515625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="28.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3551,11 +3550,8 @@
       <c r="Z1" s="16" t="s">
         <v>483</v>
       </c>
-      <c r="AA1" s="16" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>621</v>
       </c>
@@ -3630,9 +3626,8 @@
       <c r="Z2" s="19" t="s">
         <v>636</v>
       </c>
-      <c r="AA2" s="19"/>
-    </row>
-    <row r="3" spans="1:27" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>622</v>
       </c>
@@ -3711,9 +3706,8 @@
       <c r="Z3" s="19" t="s">
         <v>674</v>
       </c>
-      <c r="AA3" s="19"/>
-    </row>
-    <row r="4" spans="1:27" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>624</v>
       </c>
@@ -3788,9 +3782,8 @@
       <c r="Z4" s="19" t="s">
         <v>642</v>
       </c>
-      <c r="AA4" s="17"/>
-    </row>
-    <row r="5" spans="1:27" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>627</v>
       </c>
@@ -3867,9 +3860,8 @@
       <c r="Z5" s="17" t="s">
         <v>647</v>
       </c>
-      <c r="AA5" s="17"/>
-    </row>
-    <row r="6" spans="1:27" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>679</v>
       </c>
@@ -3944,39 +3936,38 @@
       <c r="Z6" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="AA6" s="17"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="M7" s="17"/>
       <c r="V7" s="22"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K8" s="17"/>
       <c r="M8" s="17"/>
       <c r="V8" s="22"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
       <c r="V9" s="22"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L10" s="17"/>
       <c r="V10" s="22"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O11" s="20"/>
       <c r="V11" s="22"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K12" s="17"/>
       <c r="V12" s="22"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K13" s="17"/>
       <c r="V13" s="22"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="J14" s="17"/>
       <c r="V14" s="22"/>
     </row>
@@ -4125,7 +4116,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Z1:AA1</xm:sqref>
+          <xm:sqref>Z1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>

</xml_diff>

<commit_message>
Started all OLR wrangling, normalized and reconciled names and subjects
</commit_message>
<xml_diff>
--- a/datamares/OLR/OLR_datamares_ecosystems.xlsx
+++ b/datamares/OLR/OLR_datamares_ecosystems.xlsx
@@ -1919,9 +1919,6 @@
     <t>Vanderplank, Sula</t>
   </si>
   <si>
-    <t>Cabo Pulmo National Park</t>
-  </si>
-  <si>
     <t>2014 to 2015</t>
   </si>
   <si>
@@ -1940,9 +1937,6 @@
     <t>2016-12-31</t>
   </si>
   <si>
-    <t>Gulf of California</t>
-  </si>
-  <si>
     <t>Satellite and bibliographic</t>
   </si>
   <si>
@@ -1958,9 +1952,6 @@
     <t>Mapping Ocean's Wealth - Habitats extent</t>
   </si>
   <si>
-    <t>Mangroves | Sargassum | Corals | Rocky reef | Seamounts | Habitats</t>
-  </si>
-  <si>
     <t>2016-07-25</t>
   </si>
   <si>
@@ -1968,9 +1959,6 @@
   </si>
   <si>
     <t>Marine habitat distributions in the Gulf of California @ http://dx.doi.org/10.13022/M3S59N</t>
-  </si>
-  <si>
-    <t>Climate change | Pollution | Marine protected areas | Global</t>
   </si>
   <si>
     <t>2016-06-19</t>
@@ -2044,22 +2032,10 @@
     <t>Plankton tows, DNA analysis, genetic barcoding</t>
   </si>
   <si>
-    <t>Habitat complexity | Fish | Genetics</t>
-  </si>
-  <si>
-    <t>Cabo Pulmo National Park | Baja California Sur | Mexico | Gulf of California</t>
-  </si>
-  <si>
     <t>Exploring diversity in Cabo Pulmo National Park through fish eggs and larvae @ http://dx.doi.org/10.13022/M3KK5D</t>
   </si>
   <si>
     <t>ec_cp_fish_larvae.xlsx</t>
-  </si>
-  <si>
-    <t>El Niño Southern Oscillation | Temperature | Chlorophyll a | Ecosystem | Oceans</t>
-  </si>
-  <si>
-    <t>Endemic | Norma Oficial Mexicana (NOM) | Protected | Habitats</t>
   </si>
   <si>
     <r>
@@ -2118,6 +2094,30 @@
   </si>
   <si>
     <t>Ahern, Ana Luisa; Burton, Ron; Gomez, Jaime; Aburto-Oropeza, Octavio (20##): Exploring diversity in Cabo Pulmo National Park through fish eggs and larvae. In dataMares Project: Ecosystem Dynamics. UC San Diego Library Digital Collections.</t>
+  </si>
+  <si>
+    <t>California, Gulf of (Mexico)</t>
+  </si>
+  <si>
+    <t>Cabo Pulmo National Park (Mexico)</t>
+  </si>
+  <si>
+    <t>Cabo Pulmo National Park (Mexico) | Baja California Sur (Mexico) | Mexico | California, Gulf of (Mexico)</t>
+  </si>
+  <si>
+    <t>Endemic animals | Norma Oficial Mexicana (NOM) | Protected wildlands | Habitats</t>
+  </si>
+  <si>
+    <t>Fish | Genetics</t>
+  </si>
+  <si>
+    <t>El Niño Southern Oscillation | Ocean temperature | Chlorophyll a | Ecosystem | Ocean</t>
+  </si>
+  <si>
+    <t>Mangrove | Sargassum | Coral | Rocky reef | Seamount | Endemic animals</t>
+  </si>
+  <si>
+    <t>Climate change | Marine pollution | Marine protected area | Global</t>
   </si>
 </sst>
 </file>
@@ -3439,10 +3439,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="Y4" sqref="Y4"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,7 +3479,7 @@
         <v>486</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>2</v>
@@ -3559,10 +3559,10 @@
         <v>485</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>403</v>
@@ -3593,38 +3593,38 @@
         <v>625</v>
       </c>
       <c r="O2" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>632</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>633</v>
       </c>
-      <c r="Q2" s="17" t="s">
-        <v>634</v>
-      </c>
       <c r="R2" s="22" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="S2" s="29"/>
       <c r="T2" s="22" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="V2" s="22" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="W2" s="22" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>631</v>
+        <v>684</v>
       </c>
       <c r="Z2" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3635,10 +3635,10 @@
         <v>485</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>403</v>
@@ -3653,10 +3653,10 @@
         <v>433</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="K3" s="17" t="s">
         <v>626</v>
@@ -3668,43 +3668,43 @@
         <v>623</v>
       </c>
       <c r="N3" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>672</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>662</v>
+      </c>
+      <c r="S3" s="29" t="s">
+        <v>682</v>
+      </c>
+      <c r="T3" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>665</v>
+      </c>
+      <c r="V3" s="22" t="s">
         <v>666</v>
       </c>
-      <c r="O3" s="17" t="s">
-        <v>680</v>
-      </c>
-      <c r="P3" s="17" t="s">
+      <c r="W3" s="22" t="s">
         <v>667</v>
       </c>
-      <c r="Q3" s="17" t="s">
-        <v>637</v>
-      </c>
-      <c r="R3" s="22" t="s">
-        <v>666</v>
-      </c>
-      <c r="S3" s="29" t="s">
-        <v>690</v>
-      </c>
-      <c r="T3" s="22" t="s">
+      <c r="X3" s="17" t="s">
+        <v>687</v>
+      </c>
+      <c r="Y3" s="17" t="s">
+        <v>685</v>
+      </c>
+      <c r="Z3" s="19" t="s">
         <v>668</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>669</v>
-      </c>
-      <c r="V3" s="22" t="s">
-        <v>670</v>
-      </c>
-      <c r="W3" s="22" t="s">
-        <v>671</v>
-      </c>
-      <c r="X3" s="17" t="s">
-        <v>672</v>
-      </c>
-      <c r="Y3" s="17" t="s">
-        <v>673</v>
-      </c>
-      <c r="Z3" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3715,10 +3715,10 @@
         <v>485</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>403</v>
@@ -3733,7 +3733,7 @@
         <v>433</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>626</v>
@@ -3752,35 +3752,35 @@
         <v>625</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="S4" s="29"/>
       <c r="T4" s="22" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="U4" s="21" t="s">
+        <v>651</v>
+      </c>
+      <c r="V4" s="22" t="s">
         <v>655</v>
       </c>
-      <c r="V4" s="22" t="s">
-        <v>659</v>
-      </c>
       <c r="W4" s="22" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="X4" s="17" t="s">
-        <v>676</v>
+        <v>688</v>
       </c>
       <c r="Y4" s="17" t="s">
-        <v>638</v>
+        <v>683</v>
       </c>
       <c r="Z4" s="19" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3791,10 +3791,10 @@
         <v>485</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>403</v>
@@ -3809,10 +3809,10 @@
         <v>433</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>626</v>
@@ -3827,52 +3827,52 @@
         <v>625</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="Q5" s="17" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="R5" s="22" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="S5" s="29"/>
       <c r="T5" s="22" t="s">
+        <v>675</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="W5" s="22" t="s">
+        <v>653</v>
+      </c>
+      <c r="X5" s="17" t="s">
+        <v>689</v>
+      </c>
+      <c r="Y5" s="17" t="s">
         <v>683</v>
       </c>
-      <c r="U5" s="22" t="s">
-        <v>656</v>
-      </c>
-      <c r="V5" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="W5" s="22" t="s">
-        <v>657</v>
-      </c>
-      <c r="X5" s="17" t="s">
+      <c r="Z5" s="17" t="s">
         <v>644</v>
-      </c>
-      <c r="Y5" s="17" t="s">
-        <v>638</v>
-      </c>
-      <c r="Z5" s="17" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>485</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>403</v>
@@ -3887,10 +3887,10 @@
         <v>433</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>626</v>
@@ -3905,36 +3905,36 @@
         <v>625</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="Q6" s="17" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="S6" s="29"/>
       <c r="T6" s="22" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="U6" s="22" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="V6" s="22" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="W6" s="24" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="X6" s="17" t="s">
-        <v>648</v>
+        <v>690</v>
       </c>
       <c r="Y6" s="17"/>
       <c r="Z6" s="17" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -4091,7 +4091,7 @@
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="1495" yWindow="249" count="2">
+  <dataValidations disablePrompts="1" xWindow="1495" yWindow="249" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list" sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="G1:H1"/>
   </dataValidations>
@@ -4099,7 +4099,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1495" yWindow="249" count="12">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="1495" yWindow="249" count="12">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>

</xml_diff>

<commit_message>
Stripped 'Embargo Date' column from OLRs
</commit_message>
<xml_diff>
--- a/datamares/OLR/OLR_datamares_ecosystems.xlsx
+++ b/datamares/OLR/OLR_datamares_ecosystems.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="688">
   <si>
     <t>text</t>
   </si>
@@ -1995,15 +1995,6 @@
   </si>
   <si>
     <t>Software used: Microsoft Excel, Tableau. Coordinate system: WGS1984.</t>
-  </si>
-  <si>
-    <t>EMBARGO DATE</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>2019-01-01</t>
   </si>
   <si>
     <t>Exploring diversity in Cabo Pulmo National Park through fish eggs and larvae</t>
@@ -3437,41 +3428,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.140625" style="25" customWidth="1"/>
-    <col min="19" max="19" width="39.140625" style="29" customWidth="1"/>
-    <col min="20" max="20" width="39.140625" style="25" customWidth="1"/>
-    <col min="21" max="21" width="33" style="25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="39.140625" style="25" customWidth="1"/>
-    <col min="23" max="23" width="34.85546875" style="25" customWidth="1"/>
-    <col min="24" max="25" width="42.85546875" style="3" customWidth="1"/>
-    <col min="26" max="26" width="59.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.140625" style="25" customWidth="1"/>
+    <col min="18" max="18" width="39.140625" style="29" customWidth="1"/>
+    <col min="19" max="19" width="39.140625" style="25" customWidth="1"/>
+    <col min="20" max="20" width="33" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.140625" style="25" customWidth="1"/>
+    <col min="22" max="22" width="34.85546875" style="25" customWidth="1"/>
+    <col min="23" max="24" width="42.85546875" style="3" customWidth="1"/>
+    <col min="25" max="25" width="59.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3479,79 +3469,76 @@
         <v>486</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>657</v>
+        <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="15" t="s">
         <v>1</v>
       </c>
+      <c r="I1" s="16" t="s">
+        <v>284</v>
+      </c>
       <c r="J1" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="K1" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>105</v>
       </c>
+      <c r="L1" s="16" t="s">
+        <v>105</v>
+      </c>
       <c r="M1" s="16" t="s">
-        <v>105</v>
+        <v>450</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>450</v>
+        <v>489</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>489</v>
+        <v>6</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="Q1" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="R1" s="28" t="s">
         <v>352</v>
       </c>
+      <c r="S1" s="23" t="s">
+        <v>4</v>
+      </c>
       <c r="T1" s="23" t="s">
-        <v>4</v>
+        <v>354</v>
       </c>
       <c r="U1" s="23" t="s">
-        <v>354</v>
+        <v>507</v>
       </c>
       <c r="V1" s="23" t="s">
-        <v>507</v>
-      </c>
-      <c r="W1" s="23" t="s">
         <v>506</v>
       </c>
+      <c r="W1" s="16" t="s">
+        <v>460</v>
+      </c>
       <c r="X1" s="16" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="Y1" s="16" t="s">
-        <v>455</v>
-      </c>
-      <c r="Z1" s="16" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>621</v>
       </c>
@@ -3559,75 +3546,72 @@
         <v>485</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>658</v>
+        <v>634</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>634</v>
+        <v>403</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>403</v>
+        <v>473</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>473</v>
+        <v>358</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>358</v>
+        <v>433</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>433</v>
+        <v>629</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>630</v>
-      </c>
-      <c r="K2" s="17" t="s">
         <v>626</v>
       </c>
-      <c r="L2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17" t="s">
+        <v>623</v>
+      </c>
       <c r="M2" s="17" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>632</v>
-      </c>
-      <c r="Q2" s="17" t="s">
         <v>633</v>
       </c>
-      <c r="R2" s="22" t="s">
-        <v>678</v>
-      </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="22" t="s">
-        <v>673</v>
-      </c>
-      <c r="U2" s="21" t="s">
+      <c r="Q2" s="22" t="s">
+        <v>675</v>
+      </c>
+      <c r="R2" s="29"/>
+      <c r="S2" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="T2" s="21" t="s">
         <v>650</v>
       </c>
+      <c r="U2" s="22" t="s">
+        <v>655</v>
+      </c>
       <c r="V2" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="W2" s="22" t="s">
         <v>649</v>
       </c>
+      <c r="W2" s="17" t="s">
+        <v>683</v>
+      </c>
       <c r="X2" s="17" t="s">
-        <v>686</v>
-      </c>
-      <c r="Y2" s="17" t="s">
-        <v>684</v>
-      </c>
-      <c r="Z2" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y2" s="19" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>622</v>
       </c>
@@ -3635,79 +3619,76 @@
         <v>485</v>
       </c>
       <c r="C3" s="17" t="s">
+        <v>666</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>657</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>626</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>628</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>623</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>659</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="N3" s="17" t="s">
         <v>669</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>358</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>433</v>
-      </c>
-      <c r="I3" s="17" t="s">
+      <c r="O3" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="P3" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>659</v>
+      </c>
+      <c r="R3" s="29" t="s">
+        <v>679</v>
+      </c>
+      <c r="S3" s="22" t="s">
         <v>661</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>626</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>628</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>623</v>
-      </c>
-      <c r="N3" s="17" t="s">
+      <c r="T3" s="21" t="s">
         <v>662</v>
       </c>
-      <c r="O3" s="17" t="s">
-        <v>672</v>
-      </c>
-      <c r="P3" s="17" t="s">
+      <c r="U3" s="22" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="17" t="s">
-        <v>636</v>
-      </c>
-      <c r="R3" s="22" t="s">
-        <v>662</v>
-      </c>
-      <c r="S3" s="29" t="s">
+      <c r="V3" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="W3" s="17" t="s">
+        <v>684</v>
+      </c>
+      <c r="X3" s="17" t="s">
         <v>682</v>
       </c>
-      <c r="T3" s="22" t="s">
-        <v>664</v>
-      </c>
-      <c r="U3" s="21" t="s">
+      <c r="Y3" s="19" t="s">
         <v>665</v>
       </c>
-      <c r="V3" s="22" t="s">
-        <v>666</v>
-      </c>
-      <c r="W3" s="22" t="s">
-        <v>667</v>
-      </c>
-      <c r="X3" s="17" t="s">
-        <v>687</v>
-      </c>
-      <c r="Y3" s="17" t="s">
-        <v>685</v>
-      </c>
-      <c r="Z3" s="19" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:25" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>624</v>
       </c>
@@ -3715,75 +3696,72 @@
         <v>485</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>658</v>
+        <v>638</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>638</v>
+        <v>403</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>403</v>
+        <v>473</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>473</v>
+        <v>358</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>358</v>
+        <v>433</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>433</v>
+        <v>667</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>670</v>
+        <v>626</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>626</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>626</v>
-      </c>
-      <c r="L4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17" t="s">
+        <v>623</v>
+      </c>
       <c r="M4" s="17" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="N4" s="17" t="s">
         <v>625</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>625</v>
+        <v>639</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>639</v>
-      </c>
-      <c r="Q4" s="17" t="s">
         <v>636</v>
       </c>
-      <c r="R4" s="22" t="s">
-        <v>679</v>
-      </c>
-      <c r="S4" s="29"/>
-      <c r="T4" s="22" t="s">
-        <v>674</v>
-      </c>
-      <c r="U4" s="21" t="s">
+      <c r="Q4" s="22" t="s">
+        <v>676</v>
+      </c>
+      <c r="R4" s="29"/>
+      <c r="S4" s="22" t="s">
+        <v>671</v>
+      </c>
+      <c r="T4" s="21" t="s">
         <v>651</v>
       </c>
+      <c r="U4" s="22" t="s">
+        <v>655</v>
+      </c>
       <c r="V4" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="W4" s="22" t="s">
         <v>637</v>
       </c>
+      <c r="W4" s="17" t="s">
+        <v>685</v>
+      </c>
       <c r="X4" s="17" t="s">
-        <v>688</v>
-      </c>
-      <c r="Y4" s="17" t="s">
-        <v>683</v>
-      </c>
-      <c r="Z4" s="19" t="s">
+        <v>680</v>
+      </c>
+      <c r="Y4" s="19" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>627</v>
       </c>
@@ -3791,40 +3769,40 @@
         <v>485</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>643</v>
+        <v>403</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>403</v>
+        <v>473</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>473</v>
+        <v>358</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>358</v>
+        <v>433</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>433</v>
+        <v>641</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>641</v>
+        <v>674</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>677</v>
+        <v>626</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>625</v>
+        <v>642</v>
       </c>
       <c r="O5" s="17" t="s">
         <v>642</v>
@@ -3832,77 +3810,74 @@
       <c r="P5" s="17" t="s">
         <v>642</v>
       </c>
-      <c r="Q5" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="R5" s="22" t="s">
+      <c r="Q5" s="22" t="s">
+        <v>677</v>
+      </c>
+      <c r="R5" s="29"/>
+      <c r="S5" s="22" t="s">
+        <v>672</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>653</v>
+      </c>
+      <c r="W5" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="X5" s="17" t="s">
         <v>680</v>
       </c>
-      <c r="S5" s="29"/>
-      <c r="T5" s="22" t="s">
-        <v>675</v>
-      </c>
-      <c r="U5" s="22" t="s">
-        <v>652</v>
-      </c>
-      <c r="V5" s="22" t="s">
-        <v>656</v>
-      </c>
-      <c r="W5" s="22" t="s">
-        <v>653</v>
-      </c>
-      <c r="X5" s="17" t="s">
-        <v>689</v>
-      </c>
       <c r="Y5" s="17" t="s">
-        <v>683</v>
-      </c>
-      <c r="Z5" s="17" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>485</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>658</v>
+        <v>646</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>646</v>
+        <v>403</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>403</v>
+        <v>473</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>473</v>
+        <v>358</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>358</v>
+        <v>433</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>433</v>
+        <v>654</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>677</v>
+        <v>626</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="O6" s="17" t="s">
         <v>645</v>
@@ -3910,66 +3885,63 @@
       <c r="P6" s="17" t="s">
         <v>645</v>
       </c>
-      <c r="Q6" s="17" t="s">
-        <v>645</v>
-      </c>
-      <c r="R6" s="22" t="s">
-        <v>681</v>
-      </c>
-      <c r="S6" s="29"/>
+      <c r="Q6" s="22" t="s">
+        <v>678</v>
+      </c>
+      <c r="R6" s="29"/>
+      <c r="S6" s="22" t="s">
+        <v>673</v>
+      </c>
       <c r="T6" s="22" t="s">
-        <v>676</v>
+        <v>652</v>
       </c>
       <c r="U6" s="22" t="s">
-        <v>652</v>
-      </c>
-      <c r="V6" s="22" t="s">
         <v>655</v>
       </c>
-      <c r="W6" s="24" t="s">
+      <c r="V6" s="24" t="s">
         <v>647</v>
       </c>
-      <c r="X6" s="17" t="s">
-        <v>690</v>
-      </c>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17" t="s">
+      <c r="W6" s="17" t="s">
+        <v>687</v>
+      </c>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="M7" s="17"/>
-      <c r="V7" s="22"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="V8" s="22"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L7" s="17"/>
+      <c r="U7" s="22"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="U8" s="22"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J9" s="17"/>
       <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="V9" s="22"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="L10" s="17"/>
-      <c r="V10" s="22"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O11" s="20"/>
-      <c r="V11" s="22"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K12" s="17"/>
-      <c r="V12" s="22"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K13" s="17"/>
-      <c r="V13" s="22"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="J14" s="17"/>
-      <c r="V14" s="22"/>
+      <c r="U9" s="22"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K10" s="17"/>
+      <c r="U10" s="22"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N11" s="20"/>
+      <c r="U11" s="22"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J12" s="17"/>
+      <c r="U12" s="22"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J13" s="17"/>
+      <c r="U13" s="22"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I14" s="17"/>
+      <c r="U14" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B1048576 B1:B2 B4:B7">
@@ -4093,7 +4065,7 @@
   </conditionalFormatting>
   <dataValidations disablePrompts="1" xWindow="1495" yWindow="249" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="G1:H1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="F1:G1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4104,31 +4076,31 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>I1</xm:sqref>
+          <xm:sqref>H1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>N1:O1</xm:sqref>
+          <xm:sqref>M1:N1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Z1</xm:sqref>
+          <xm:sqref>Y1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>E2 E4:E1048576</xm:sqref>
+          <xm:sqref>D2 D4:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
           </x14:formula1>
-          <xm:sqref>F2 F4:F1048576</xm:sqref>
+          <xm:sqref>E2 E4:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
@@ -4140,37 +4112,37 @@
           <x14:formula1>
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:H2 G4:H1048576</xm:sqref>
+          <xm:sqref>F2:G2 F4:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'[1]CV values'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:H3</xm:sqref>
+          <xm:sqref>F3:G3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'[1]CV values'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B3 E3:F3</xm:sqref>
+          <xm:sqref>B3 D3:E3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$13</xm:f>
           </x14:formula1>
-          <xm:sqref>X1:Y1</xm:sqref>
+          <xm:sqref>W1:X1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$30</xm:f>
           </x14:formula1>
-          <xm:sqref>R1:W1</xm:sqref>
+          <xm:sqref>Q1:V1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$B$1:$B$233</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:K1</xm:sqref>
+          <xm:sqref>I1:J1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fixed broken DOI in promonitor OLR and added ecosystems OLR for test ingest
</commit_message>
<xml_diff>
--- a/datamares/OLR/OLR_datamares_ecosystems.xlsx
+++ b/datamares/OLR/OLR_datamares_ecosystems.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="687">
   <si>
     <t>text</t>
   </si>
@@ -2024,9 +2024,6 @@
   </si>
   <si>
     <t>Exploring diversity in Cabo Pulmo National Park through fish eggs and larvae @ http://dx.doi.org/10.13022/M3KK5D</t>
-  </si>
-  <si>
-    <t>ec_cp_fish_larvae.xlsx</t>
   </si>
   <si>
     <r>
@@ -3433,7 +3430,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,11 +3583,11 @@
         <v>633</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="R2" s="29"/>
       <c r="S2" s="22" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="T2" s="21" t="s">
         <v>650</v>
@@ -3602,10 +3599,10 @@
         <v>649</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="Y2" s="19" t="s">
         <v>635</v>
@@ -3618,15 +3615,9 @@
       <c r="B3" s="17" t="s">
         <v>485</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>666</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>473</v>
-      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="17" t="s">
         <v>358</v>
       </c>
@@ -3652,7 +3643,7 @@
         <v>659</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O3" s="17" t="s">
         <v>660</v>
@@ -3664,7 +3655,7 @@
         <v>659</v>
       </c>
       <c r="R3" s="29" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="S3" s="22" t="s">
         <v>661</v>
@@ -3679,10 +3670,10 @@
         <v>664</v>
       </c>
       <c r="W3" s="17" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="X3" s="17" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="Y3" s="19" t="s">
         <v>665</v>
@@ -3711,7 +3702,7 @@
         <v>433</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>626</v>
@@ -3736,11 +3727,11 @@
         <v>636</v>
       </c>
       <c r="Q4" s="22" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="R4" s="29"/>
       <c r="S4" s="22" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="T4" s="21" t="s">
         <v>651</v>
@@ -3752,10 +3743,10 @@
         <v>637</v>
       </c>
       <c r="W4" s="17" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="X4" s="17" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="Y4" s="19" t="s">
         <v>640</v>
@@ -3787,7 +3778,7 @@
         <v>641</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>626</v>
@@ -3811,11 +3802,11 @@
         <v>642</v>
       </c>
       <c r="Q5" s="22" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="R5" s="29"/>
       <c r="S5" s="22" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="T5" s="22" t="s">
         <v>652</v>
@@ -3827,10 +3818,10 @@
         <v>653</v>
       </c>
       <c r="W5" s="17" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="X5" s="17" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="Y5" s="17" t="s">
         <v>644</v>
@@ -3838,7 +3829,7 @@
     </row>
     <row r="6" spans="1:25" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>485</v>
@@ -3862,7 +3853,7 @@
         <v>654</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>626</v>
@@ -3886,11 +3877,11 @@
         <v>645</v>
       </c>
       <c r="Q6" s="22" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="R6" s="29"/>
       <c r="S6" s="22" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="T6" s="22" t="s">
         <v>652</v>
@@ -3902,7 +3893,7 @@
         <v>647</v>
       </c>
       <c r="W6" s="17" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="X6" s="17"/>
       <c r="Y6" s="17" t="s">

</xml_diff>